<commit_message>
more board desings, and arduino code
</commit_message>
<xml_diff>
--- a/boards/unoshield-v5-bom.xlsx
+++ b/boards/unoshield-v5-bom.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22325"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lafel\OneDrive\Documents\GitHub\trashrobot5\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lafel\OneDrive\Documents\GitHub\trashrobot5\boards\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="35" documentId="8_{786209F5-C015-42DF-8439-BD069CB84789}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D9BA65F3-ADE5-425B-B3E3-DC15DD47CEC7}"/>
@@ -795,7 +795,7 @@
   <dimension ref="A1:I45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+      <selection activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>

</xml_diff>